<commit_message>
Fixed phrasing for some of the column descriptions
</commit_message>
<xml_diff>
--- a/data/Metadata_AmphiTherm.xlsx
+++ b/data/Metadata_AmphiTherm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/10bd42275f629cc1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5288536_ad_unsw_edu_au/Documents/[ PhD UNSW ]/Side project - Database amphibian CTmin and Tpref/AmphiTherm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C60EEDF2-2807-41ED-92EF-5B479B3DF176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{C60EEDF2-2807-41ED-92EF-5B479B3DF176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE2ED6F-1910-4D59-9DDD-ED953A7B91CA}"/>
   <bookViews>
-    <workbookView xWindow="-9540" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{6B4B34E7-B746-4674-8CD6-5684642F9B01}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6B4B34E7-B746-4674-8CD6-5684642F9B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,15 +53,9 @@
     <t>ref</t>
   </si>
   <si>
-    <t>Abbreviated reference for the study, using Author_et_al_DATE (usually the name of the PDF file). E.g., “Simon_et_al_2015“</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
-    <t xml:space="preserve">Title of the paper. </t>
-  </si>
-  <si>
     <t>doi</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>strain</t>
   </si>
   <si>
-    <t>The strain, variety, subspecies, or morph of the species, if reported in the study.</t>
-  </si>
-  <si>
     <t>origin</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>sex</t>
   </si>
   <si>
-    <t>The sex of the animals. Factor with four levels: “male”, “female”, “mixed”, “unknown”. The “mixed” category is used when authors clearly stipulate that they mixed males and females.</t>
-  </si>
-  <si>
     <t>metric</t>
   </si>
   <si>
@@ -210,9 +198,6 @@
   </si>
   <si>
     <t>n_replicates_per_temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If the metric was LT50, the number of replicates used at each test temperatures. E.g., if authors used 5 test temperatures and measured the survival of three independent cohorts of animals at each test temperature, then n_replicates_per_temp = 3. Numeric values only. </t>
   </si>
   <si>
     <t>n_animals_per_replicate</t>
@@ -311,9 +296,6 @@
     <t>unique_ID</t>
   </si>
   <si>
-    <t>Unique identifier for each observation (e.g., 1,2,3,4)</t>
-  </si>
-  <si>
     <t>thesis_chapter</t>
   </si>
   <si>
@@ -323,15 +305,9 @@
     <t>For theses, the title of the chapter from which the data were extracted.</t>
   </si>
   <si>
-    <t>For theses, the chapter of the thesis from which the data were extracted.</t>
-  </si>
-  <si>
     <t>peer-reviewed</t>
   </si>
   <si>
-    <t>Whether the study was published in journals or was a thesis. Factor with two levels: "peer-reviewed" and "not_peer-reviewed".</t>
-  </si>
-  <si>
     <t>notes_ID</t>
   </si>
   <si>
@@ -344,159 +320,37 @@
     <t>pub_year</t>
   </si>
   <si>
-    <t>Publication year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique identifier for each cohort. By “cohort”, we designate independent groups of animals. In some cases, traits can be measured multiple times on the same cohort of animals (e.g. using different endpoints, or at different ages). As such, the same cohort_ID was used for repeated measures. The cohort_ID is structured as a combination of the species name, the population number, the trait, and the cohort number (e.g., Eupemphix_nattereri_pop1_UTL_co1). </t>
-  </si>
-  <si>
     <t>order</t>
   </si>
   <si>
-    <t>Species order, according to AmphibiaWeb (https://amphibiaweb.org/taxonomy/index.html)</t>
-  </si>
-  <si>
-    <t>Species family, according to AmphibiaWeb (https://amphibiaweb.org/taxonomy/index.html)</t>
-  </si>
-  <si>
-    <t>Species binomial nomenclature, according to AmphibiaWeb (https://amphibiaweb.org/taxonomy/index.html)</t>
-  </si>
-  <si>
     <t>IUCN_status</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique identifier for each population. We refer to distinctions between populations made by the authors (e.g., “northern population”, “central population”, and “south population").  Note that when multiple data points were extracted from the same population, they shared the same population_ID. The population_ID is structured as a combination of the species name and the population number (e.g., Eupemphix_nattereri_pop1). </t>
-  </si>
-  <si>
-    <t>Threat status, according to the International Union for the Conservation of Nature (IUCN). Factor with 8 levels: DD (data-deficient), LC (least-concern), NT (near threatened), VU (vulnerable), EN (endangered), CR (critically endangered), EXW (extinct in the wild), and EX (exctinct).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Origin of studied animals. Factor with two levels: recently collected from the wild (i.e. “wild”) or eggs laid in the laboratory (i.e. “lab”). For studies collecting eggs from the wild and testing the same generation of animals, they were considered as “wild”. </t>
-  </si>
-  <si>
-    <t>Latitude from which animals were collected (decimal degrees). If animals were collected at various latitudes and the data was not reported separately for each population (and if the raw data is not published) the mean of the different latitudes reported was taken.</t>
-  </si>
-  <si>
-    <t>Longitude from which animals were collected (decimal degrees). If animals were collected at various longitudes and the data was not reported separately for each population (and if the raw data is not published) the mean of the different longitude reported was taken.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Latitude from which animals were collected (degrees, minutes, seconds; e.g. 41,42,26.33N). If the latitude was already reported in decimal degrees, this column was left blank. </t>
   </si>
   <si>
     <t xml:space="preserve">Longitude from which animals were collected (degrees, minutes, seconds; e.g. 80,21,09.03W).  If the longitude was already reported in decimal degrees, this column was left blank. </t>
   </si>
   <si>
-    <t>Elevation from which animals were collected (meters above sea level), as reported in the study. If not reported in the study, this was estimated using https://www.freemaptools.com/elevation-finder.htm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date at which the animals were sampled (format YEAR/MONTH/DAY, e.g. “2020/07/26”). If the precise day is not reported, the month was reported in “month_sampling”. If a range of dates was presented (e.g., “June to August 2020”),  details were reported in the “start range_sampling_dates” and “end_range_sampling_dates” columns. </t>
-  </si>
-  <si>
     <t>Month from which the animals were collected. If the sampling spans two or more months, details were reported in the “start_range_sampling_dates” and “end_range_sampling_dates” columns.</t>
   </si>
   <si>
     <t xml:space="preserve">Year from which the animals were collected. If the sampling spanned two years, details were reported in the “start_range_sampling_dates” and “end_range_sampling_dates” columns. </t>
   </si>
   <si>
-    <t xml:space="preserve">The beginning of the range of dates over which animals were collected (e.g. “January_2015”). </t>
-  </si>
-  <si>
-    <t>The end of the range of dates over which animals were collected (e.g. “September_2015”).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional comments regarding the sampling of the animals. E.g. if animals were sampled on a non-continuous scale (e.g. in July 2015, May 2016, and September 2016). </t>
-  </si>
-  <si>
     <t>notes_sampling</t>
   </si>
   <si>
-    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean ambient temperature (°C) in the month of collection, if reported in the study. If animals were collected over a range of months, the mean temperature across this sampling period was taken.</t>
-  </si>
-  <si>
-    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean temperature of the substrate (°C) in the month of capture, if reported in the study.  If animals were collected over a range of months, the mean temperature across this sampling period was taken.</t>
-  </si>
-  <si>
-    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean water temperature (°C) in the month of collection, if reported in the study.   If animals were collected over a range of months, the mean temperature across this sampling period was taken.</t>
-  </si>
-  <si>
-    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean body temperature (°C) measured in the field when animals were collected, if reported in the study.   If animals were collected over a range of months, the mean temperature across this sampling period was taken.</t>
-  </si>
-  <si>
     <t>notes_env_temp</t>
   </si>
   <si>
-    <t>Additional comments regarding the environmental temperatures when animals were sampled.</t>
-  </si>
-  <si>
-    <r>
-      <t>Whether the animals were maintained in the laboratory for some period, or tested shortly</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> after collection. Factor with two levels: “acclimated” or “field-fresh”. </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">For animals born in the laboratory, the mean temperature (°C) at which the embryos were incubated, if reported in the study. For the temperature at which the larvae and adults were acclimated, see “acclimation_temp”. </t>
   </si>
   <si>
     <t xml:space="preserve">Variability (e.g., +/- 1C) in incubation_temp (°C), if reported. </t>
   </si>
   <si>
-    <t xml:space="preserve">For acclimated animals, the life stage acclimated prior to the thermal tolerance or preference assay. Factor with five levels: “embryos_and_larvae”, "larvae", “juveniles”, "metamorphs" or “adults”. </t>
-  </si>
-  <si>
-    <t>For acclimated animals, the Gosner stage when the acclimation started, if reported in the study. If a range of Gosner stage is presented (24-27), the mean of the range was taken.</t>
-  </si>
-  <si>
-    <t>For acclimated animals, the mean temperature of acclimation (°C). If embryos were incubated at a temperature and animals were tested upon hatching, the temperature of incubation was reported here.</t>
-  </si>
-  <si>
-    <t>The duration of acclimation (days). Numeric values only. If a range of days is presented (4-7 days), the mean of the range was used.</t>
-  </si>
-  <si>
-    <t>The life stage tested for heat tolerance.  Factor with four levels: “larvae”, "juveniles", "metamorphs, or “adults”.</t>
-  </si>
-  <si>
-    <t>Gosner stage when the animals were assessed for heat tolerance, if reported in the study. If a range of Gosner stage is presented (24-27), the mean of the range was taken.</t>
-  </si>
-  <si>
     <t>notes_acclimation</t>
-  </si>
-  <si>
-    <t>Additional comments regarding the acclimation of the animals.</t>
-  </si>
-  <si>
-    <t>Mean snout-vent length of the animals (mm) when assessed for cold tolerance, if reported in the study. Note that some of these observations were also taken from Rohr et al. 2018. Ecol. Lett.</t>
-  </si>
-  <si>
-    <t>Mean body mass of the animals (g) when assessed for cold tolerance, if reported in the study.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The age (days-post-hatching) at which the animals were tested for cold tolerance. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The metric used to assess thermal tolerance (CTmin, CTmax, LT50_cold, LT50_hot) or preferred body temperature (Tpref). Factor with five levels: “CTmin”, “LT50_cold”, "LT50_hot", "CTmax", and “Tpref”. </t>
-  </si>
-  <si>
-    <t>The endpoint that was used for assessing thermal tolerance (loss of righting response, loss of equilibrium, onset of spasms, no response to prodding, supercooling point, coma, death, other). Factor with seven levels: “LRR”, "LOE", “OS”, “prodding”, “SCP”, “coma”, “death”, “other”.</t>
-  </si>
-  <si>
-    <t>Whether the temperature measured during the thermal tolerance or preferred temperature test was the ambient, the water, the body, or substrate temperature. Factor with four levels: “ambient”, “water”, “body”, "substrate".</t>
   </si>
   <si>
     <t xml:space="preserve">If the metric was CTmin or CTmax, the starting temperature used in the thermal tolerance assay (°C). </t>
@@ -552,9 +406,6 @@
       </rPr>
       <t xml:space="preserve">°C). </t>
     </r>
-  </si>
-  <si>
-    <t>Additional comments about the thermal tolerance or preference assays.</t>
   </si>
   <si>
     <t>Humidity at which animals were acclimated or tested (% relative humidity). If the humidity during the acclimation and the test were different, priority is given to the conditions of the test.</t>
@@ -593,42 +444,24 @@
     <t xml:space="preserve">Photoperiod at which animals were acclimated (number of hours of light per day). </t>
   </si>
   <si>
-    <t>If any, which chemical (e.g. pollutant, toxin) was added to the animals’ environment. If animals were in a control group (i.e., only supplemented with a solvent),  “control” was indicated.  If no chemicals were used in the study, this field was left blank.</t>
-  </si>
-  <si>
-    <t>If any, which hormone (e.g. corticosterone, thyroid hormone) was added to the animals’ environment. If animals were in a control group (i.e., only supplemented with a solvent),  “control” was indicated.  If no hormones were used in the study, this field was left blank.</t>
-  </si>
-  <si>
     <t>If any, the concentration of the hormones or chemicals used.  If animals were in a control group, “0” was used. If no chemicals or hormones were used in the study, this field was left blank.</t>
   </si>
   <si>
-    <t>Whether the animals were infected with a pathogen. Infected animals were marked as “infected” . Otherwise, this field was left blank.</t>
-  </si>
-  <si>
     <t>Where the thermal tolerance or preferred body temperature data is reported (text, table, figure, published data).</t>
   </si>
   <si>
     <t>notes_supplements</t>
   </si>
   <si>
-    <t xml:space="preserve">Additional comments about chemicals or other supplements given to the animals. </t>
-  </si>
-  <si>
     <t>If the data was published in a repository, the url link (DOI preferred) to the repository containing the data.</t>
   </si>
   <si>
     <t>flag</t>
   </si>
   <si>
-    <t xml:space="preserve">Whether the data presents procedural inconsistencies. The exact issue is listed in this column. Note that these observations were removed from the curated version of the database. </t>
-  </si>
-  <si>
     <t>notes_trait</t>
   </si>
   <si>
-    <t>Additional comments about the thermal tolerance or preference estimates.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mean thermal tolerance or thermal preference of the animals tested (°C). </t>
   </si>
   <si>
@@ -636,6 +469,153 @@
   </si>
   <si>
     <t xml:space="preserve">Sample size of mean_trait. </t>
+  </si>
+  <si>
+    <t>Unique identifier for row in the data.</t>
+  </si>
+  <si>
+    <t>Title of the paper or thesis.</t>
+  </si>
+  <si>
+    <t>Abbreviated reference for the study.</t>
+  </si>
+  <si>
+    <t>Publication year of the paper or thesis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The title of the thesis chapter the data is taken from. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the study was peer-reviewed or not (i.e., thesis). Factor with two levels: “peer-reviewed”, “not_peer-reviewed”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique identifier for each population. Note that populations were considered individuals of the same species taken from different geographical locations.  For studies without geographical coordinates, populations were assigned based on descriptions made by the authors (e.g., “Northern population” vs. “Southern population”).  Note that when multiple data points were extracted from the same population, they shared the same population_ID. The population_ID is structured as a combination of the species name and the population number (e.g., Eupemphix_nattereri_pop1). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique identifier for each cohort. By “cohort”, we designate independent groups of animals. In some cases, traits can be measured multiple times on the same cohort of animals (e.g. using different endpoints, or at different ages). Note that cohort_ID was assigned at the trait-level; as it was not always possible to assign whether multiple traits (e.g., CTmin and CTmax) were measured with the same, or independent groups of animals.  As such, the same cohort_ID was used for repeated measures. The cohort_ID is structured as a combination of the species name, the population number, the trait, and the cohort number (e.g., Eupemphix_nattereri_pop1_UTL_co1). </t>
+  </si>
+  <si>
+    <t>Species order, according to Jetz and Pyron (2018).</t>
+  </si>
+  <si>
+    <t>Species family, according to Jetz and Pyron (2018).</t>
+  </si>
+  <si>
+    <t>Species binomial nomenclature, according to Jetz and Pyron (2018).</t>
+  </si>
+  <si>
+    <t>The strain, variety, subspecies, or morph of the species, as reported in the study.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International Union for the Conservation of Nature (IUCN) threat status. Factor with 7 levels: “DD”, “LC”, “NT”, “VU”, “EN”, “CR” and “EX”, for “data-deficient”, “least-concern”, “near threatened”, “vulnerable”, “endangered”, “critically endangered” and “extinct”, respectively.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Origin of studied animals. Factor with four levels: recently collected from the wild (i.e., “wild”), eggs laid in the laboratory (i.e., “lab”), animals provided from a supplier (i.e., “supplier”) or “unclear”. For studies collecting eggs from the wild and testing the same generation of animals, animals were considered as “wild”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude from which animals were collected (decimal degrees). Latitudes presented in degrees/minutes/seconds were converted to decimal degrees. When geographical coordinates were not presented, the coordinates were estimated using Google Maps. </t>
+  </si>
+  <si>
+    <t>Longitude from which animals were collected (decimal degrees). Longitudes presented in degrees/minutes/seconds were converted to decimal degrees. When geographical coordinates were not presented, the coordinates were estimated using Google Maps.</t>
+  </si>
+  <si>
+    <t>Elevation from which animals were collected (meters above sea level), as reported in the study. When not reported, elevation was estimated using latitude and longitude and freemaptools.com.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date at which the animals were sampled (format YEAR/MONTH/DAY, e.g. “2020/07/26”). If the precise day is not reported, the month was reported in “month_sampling”. If a range of dates was presented (e.g., “June to August 2020”), details were reported in the “start range_sampling_dates” and “end_range_sampling_dates” columns. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The beginning of the range of dates over which animals were collected. Indicated are both the month and the year of collection (e.g., “January_2015”). </t>
+  </si>
+  <si>
+    <t>The end of the range of dates over which animals were collected. Indicated are both the month and the year of collection (e.g., “September_2015”).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General notes regarding the sampling of the animals. </t>
+  </si>
+  <si>
+    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean ambient temperature (°C) in the month of collection, if reported in the study. If animals were collected over a range of months, the mean temperature across this sampling period was reported.</t>
+  </si>
+  <si>
+    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean temperature of the substrate (°C) in the month of capture.   If animals were collected over a range of months, the mean temperature across this sampling period was reported.</t>
+  </si>
+  <si>
+    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean water temperature (°C) in the month of collection. If animals were collected over a range of months, the mean temperature across this sampling period was reported.</t>
+  </si>
+  <si>
+    <t>For animals recently sampled from the wild (eggs not laid in the laboratory), the mean body temperature (°C) measured in the field when animals were collected. If animals were collected over a range of months, the mean temperature across this sampling period was reported.</t>
+  </si>
+  <si>
+    <t>General notes regarding the sampling of animals in the field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the animals were maintained in the laboratory for &gt;12h or tested shortly after collection. Factor with two levels: “acclimated” or “field-fresh”.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For acclimated animals, the life stage acclimated prior to the upper thermal limit assessment. Factor with five levels: “embryos_and_larvae”, “larvae”, “juveniles”, “metamorphs” or “adults”.  Larval stages of salamanders and tadpoles were referred to as “larvae”. Animals between Gosner stages 42 and 45 were considered “metamorphs”, while those between Gosner stage 45 and sexual maturity were considered “juveniles”.  </t>
+  </si>
+  <si>
+    <t>For acclimated animals, the Gosner stage when the acclimation started, if reported in the study. If a range of Gosner stage was presented (24-27), the mean of the range was taken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For acclimated animals, the mean temperature of acclimation (°C). Note that “acclimation” refers to a prolonged (&gt;12h) exposure to a new temperature. Therefore, cold/heat shocks or housing conditions just prior to assessing thermal tolerance or preference (e.g., 2 hours at 25°C) were not considered as “acclimation” conditions. If animals were exposed to multiple acclimation conditions (e.g., 15°C for 1 month, and then re-acclimated to 25°C for 7 days), we took the latest acclimation condition as the “acclimation_temp”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The duration of acclimation (days). </t>
+  </si>
+  <si>
+    <t>General notes regarding the laboratory acclimation of animals.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The life stage tested for thermal tolerance or preference.  Factor with four levels: “larvae”, “metamorphs”, “juveniles” or “adults”.  Larval stages of salamanders and tadpoles were referred to as “larvae”. Animals between Gosner stages 42 and 45 were considered “metamorphs”, while those between Gosner stage 45 and sexual maturity were considered “juveniles”.  </t>
+  </si>
+  <si>
+    <t>Gosner stage when the animals were assessed for heat tolerance, if reported in the study. If a range of Gosner stage was presented (24-27), the mean of the range was taken.</t>
+  </si>
+  <si>
+    <t>Mean snout-vent length of the animals (mm) when assessed for thermal tolerance or preference, if reported in the study. Note that SVL data was often taken from Rohr et al. (2018).</t>
+  </si>
+  <si>
+    <t>Mean body mass of the animals (g) when assessed for thermal tolerance or preference.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The age (days-post-hatching) at which the animals were tested for thermal tolerance or preference. </t>
+  </si>
+  <si>
+    <t>The sex of the animals. Factor with four levels: “male”, “female”, “mixed”, “unknown”. The “mixed” category was used when authors clearly stipulate that they mixed males and females.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The metric used to assess thermal tolerance (CTmax, LT50_hot, CTmin, LT50_cold) or preference (Tpref). Factor with five levels: “CTmax”, “LT50_hot”, “CTmin”, “LT50_cold”, “Tpref”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The endpoint that was used for assessing thermal tolerance (loss or righting response, loss of equilibrium, onset of spasms, no response to prodding, supercooling point, death). Factor with seven levels: “LRR”, “LOE”, “OS”, “prodding”, “SCP”, “death”, “other”. If “other”, details are reported in “notes_test” (see below).  </t>
+  </si>
+  <si>
+    <t>Whether the temperature measured during the test was the ambient, the water, the substrate, or the body temperature. Factor with three levels: “ambient”, “substrate”, “water”, “body”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the metric was LT50, the number of replicates used at each test temperatures. E.g., if authors used 5 test temperatures and measured the survival of three independent cohorts of animals at each test temperature, then n_replicates_per_temp = 3. </t>
+  </si>
+  <si>
+    <t>General notes regarding the thermal tolerance or preference assays.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If any, which chemical (e.g., pollutant, toxin) was added to the animals’ environment. If animals were in a control group (i.e., only supplemented with a solvent), “control” was indicated. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If any, which hormone (e.g., corticosterone, thyroid hormone) was added to the animals’ environment. If animals were in a control group (i.e., only supplemented with a solvent), “control” was indicated. </t>
+  </si>
+  <si>
+    <t>Whether the animals were infected with a pathogen. Infected animals were marked as “infected”. Otherwise, this field was left blank.</t>
+  </si>
+  <si>
+    <t>General notes regarding the addition of chemicals, hormones, or pathogens.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the data presents procedural concerns. The exact issue is listed in this column. Note that these observations were removed from the curated version of the database. </t>
+  </si>
+  <si>
+    <t>General notes about thermal tolerance or preference estimates</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CD37AA-DE25-4637-8059-CC7525F6C8AE}">
   <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1138,10 +1118,10 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1157,663 +1137,663 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="63" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="B13" s="4" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>58</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="38" thickBot="1" x14ac:dyDescent="0.4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>170</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>